<commit_message>
Zmiany w GPIO 2
</commit_message>
<xml_diff>
--- a/GPIO.xlsx
+++ b/GPIO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uki\Documents\Studia\mgr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA51FD1-E354-4F2B-B930-EEB5A9F19441}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D8F947-B26B-483C-916D-8D346C212A3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45" yWindow="1980" windowWidth="14400" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>3,3V</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Kontaktron GPIO 24</t>
+  </si>
+  <si>
+    <t>Przycisk GPIO 14</t>
   </si>
 </sst>
 </file>
@@ -477,7 +480,7 @@
   <dimension ref="A2:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,6 +550,9 @@
       <c r="C5">
         <v>8</v>
       </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
       <c r="F5" t="s">
         <v>21</v>
       </c>

</xml_diff>